<commit_message>
update knime workflow for transfer gropin models to fskx, including all fskx models
</commit_message>
<xml_diff>
--- a/gropin/schema/metadataschema1049.xlsx
+++ b/gropin/schema/metadataschema1049.xlsx
@@ -5239,7 +5239,7 @@
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>seq(2.4975024975025,5.5055,length.out=21)</t>
+          <t>seq(2.5025,5.4945054945055,length.out=21)</t>
         </is>
       </c>
     </row>
@@ -5301,7 +5301,7 @@
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>seq(299.7002997003,900.9,length.out=21)</t>
+          <t>seq(300.3,899.100899100899,length.out=21)</t>
         </is>
       </c>
     </row>
@@ -5339,8 +5339,8 @@
       <c r="O135" t="inlineStr">
         <is>
           <t>This dataframe consists of a number of columns 
-                            in relation to the number of variables of this
-                            model. One additional column contains the response
+                            in relation to the number of variables of this 
+                            model. One additional column contains the response 
                             surface mu_max result based on this secondary model.</t>
         </is>
       </c>

</xml_diff>

<commit_message>
update gropin todo list and finished models
Signed-off-by: Ruediger <dr.marcel.fuhrmann@gmail.com>
</commit_message>
<xml_diff>
--- a/gropin/schema/metadataschema1049.xlsx
+++ b/gropin/schema/metadataschema1049.xlsx
@@ -1476,6 +1476,11 @@
           <t>Applied and Environmental Microbiology ,  65_11_, 4921–4925</t>
         </is>
       </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>Applied and Environmental Microbiology ,  65_11_, 4921–4925</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1718,6 +1723,11 @@
           <t>String</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -5323,7 +5333,7 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>mumax</t>
+          <t>responseSurface</t>
         </is>
       </c>
       <c r="M135" t="inlineStr">

</xml_diff>